<commit_message>
Updated: Converter to match the most recent version of vulcan ncnn Updated: Converter and frames upscale use error levels
</commit_message>
<xml_diff>
--- a/GPUWaifu2K/calc_resize.xlsx
+++ b/GPUWaifu2K/calc_resize.xlsx
@@ -377,7 +377,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,42 +412,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>16000</v>
+        <v>12144</v>
       </c>
       <c r="B2" s="2">
-        <v>14144</v>
+        <v>16832</v>
       </c>
       <c r="C2" s="1">
         <v>100</v>
       </c>
       <c r="D2" s="2">
         <f>$A$2*C2/100</f>
-        <v>16000</v>
+        <v>12144</v>
       </c>
       <c r="E2" s="2">
         <f>$B$2*C2/100</f>
-        <v>14144</v>
+        <v>16832</v>
       </c>
       <c r="F2" s="1">
         <f>D2*E2</f>
-        <v>226304000</v>
+        <v>204407808</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C3" s="1">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D3" s="2">
         <f>$A$2*C3/100</f>
-        <v>15040</v>
+        <v>11901.12</v>
       </c>
       <c r="E3" s="2">
         <f>$B$2*C3/100</f>
-        <v>13295.36</v>
+        <v>16495.36</v>
       </c>
       <c r="F3" s="1">
         <f>D3*E3</f>
-        <v>199962214.40000001</v>
+        <v>196313258.80320001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -455,16 +455,16 @@
         <v>80</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ref="D4:D12" si="0">$A$2*C4/100</f>
-        <v>12800</v>
+        <f t="shared" ref="D4:D5" si="0">$A$2*C4/100</f>
+        <v>9715.2000000000007</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E12" si="1">$B$2*C4/100</f>
-        <v>11315.2</v>
+        <f t="shared" ref="E4:E5" si="1">$B$2*C4/100</f>
+        <v>13465.6</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F12" si="2">D4*E4</f>
-        <v>144834560</v>
+        <f t="shared" ref="F4:F5" si="2">D4*E4</f>
+        <v>130820997.12000002</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -473,15 +473,15 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>12000</v>
+        <v>9108</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="1"/>
-        <v>10608</v>
+        <v>12624</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="2"/>
-        <v>127296000</v>
+        <v>114979392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added: Tab for calculating max resolution for FFMpeg
</commit_message>
<xml_diff>
--- a/GPUWaifu2K/calc_resize.xlsx
+++ b/GPUWaifu2K/calc_resize.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="132" windowWidth="15300" windowHeight="8496"/>
+    <workbookView xWindow="384" yWindow="132" windowWidth="15300" windowHeight="8496" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Resize" sheetId="1" r:id="rId1"/>
+    <sheet name="FFMpeg" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Width</t>
   </si>
@@ -35,18 +35,31 @@
   <si>
     <t>HeightOut</t>
   </si>
+  <si>
+    <t>INT_MAX</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,10 +82,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,25 +426,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>12144</v>
+        <v>18464</v>
       </c>
       <c r="B2" s="2">
-        <v>16832</v>
+        <v>23328</v>
       </c>
       <c r="C2" s="1">
         <v>100</v>
       </c>
       <c r="D2" s="2">
         <f>$A$2*C2/100</f>
-        <v>12144</v>
+        <v>18464</v>
       </c>
       <c r="E2" s="2">
         <f>$B$2*C2/100</f>
-        <v>16832</v>
+        <v>23328</v>
       </c>
       <c r="F2" s="1">
         <f>D2*E2</f>
-        <v>204407808</v>
+        <v>430728192</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -439,15 +453,15 @@
       </c>
       <c r="D3" s="2">
         <f>$A$2*C3/100</f>
-        <v>11901.12</v>
+        <v>18094.72</v>
       </c>
       <c r="E3" s="2">
         <f>$B$2*C3/100</f>
-        <v>16495.36</v>
+        <v>22861.439999999999</v>
       </c>
       <c r="F3" s="1">
         <f>D3*E3</f>
-        <v>196313258.80320001</v>
+        <v>413671355.59680003</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -456,15 +470,15 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" ref="D4:D5" si="0">$A$2*C4/100</f>
-        <v>9715.2000000000007</v>
+        <v>14771.2</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" ref="E4:E5" si="1">$B$2*C4/100</f>
-        <v>13465.6</v>
+        <v>18662.400000000001</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4:F5" si="2">D4*E4</f>
-        <v>130820997.12000002</v>
+        <v>275666042.88000005</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -473,15 +487,32 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>9108</v>
+        <v>13848</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="1"/>
-        <v>12624</v>
+        <v>17496</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="2"/>
-        <v>114979392</v>
+        <v>242284608</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="1">
+        <v>68</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" ref="D6" si="3">$A$2*C6/100</f>
+        <v>12555.52</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" ref="E6" si="4">$B$2*C6/100</f>
+        <v>15863.04</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" ref="F6" si="5">D6*E6</f>
+        <v>199168715.98080003</v>
       </c>
     </row>
   </sheetData>
@@ -492,13 +523,222 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>19008</v>
+      </c>
+      <c r="B2">
+        <v>26624</v>
+      </c>
+      <c r="C2">
+        <v>95</v>
+      </c>
+      <c r="D2" s="2">
+        <f>$A$2*C2/100</f>
+        <v>18057.599999999999</v>
+      </c>
+      <c r="E2" s="2">
+        <f>$B$2*C2/100</f>
+        <v>25292.799999999999</v>
+      </c>
+      <c r="F2" s="3">
+        <f>((D2 * 8) + 1024)*(E2 + 128)</f>
+        <v>3698340003.8399997</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(F2 &lt; 2147483647,"OK","FAIL")</f>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>90</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D9" si="0">$A$2*C3/100</f>
+        <v>17107.2</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E9" si="1">$B$2*C3/100</f>
+        <v>23961.599999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F9" si="2">((D3 * 8) + 1024)*(E3 + 128)</f>
+        <v>3321512591.3600001</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G9" si="3">IF(F3 &lt; 2147483647,"OK","FAIL")</f>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>85</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>16156.8</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>22630.400000000001</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="2"/>
+        <v>2964927938.5599999</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="3"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>80</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>15206.4</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>21299.200000000001</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="2"/>
+        <v>2628586045.4400001</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="3"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>75</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>14256</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>19968</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="2"/>
+        <v>2312486912</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="3"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>70</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>13305.6</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>18636.8</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="2"/>
+        <v>2016630538.24</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>73</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>13875.84</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>19435.52</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>2191715231.3344002</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="3"/>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>72</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>13685.76</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>19169.28</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>2132543956.5823998</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>